<commit_message>
Cleaned up files and updated manuscript for submission
</commit_message>
<xml_diff>
--- a/Enzyme_kinetics/compiled_kinetics_2021-01-12.xlsx
+++ b/Enzyme_kinetics/compiled_kinetics_2021-01-12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/AromaticDiketones/Enzyme_kinetics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7A934B-7C92-F34A-B579-993ED9C494E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CA6864-BDFB-8D48-A68E-84421309180F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18520" yWindow="1020" windowWidth="23380" windowHeight="15440" xr2:uid="{A269AB31-0078-E14B-A934-EBBFA2C9B0CB}"/>
+    <workbookView xWindow="10480" yWindow="500" windowWidth="23380" windowHeight="15440" xr2:uid="{A269AB31-0078-E14B-A934-EBBFA2C9B0CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>concentration (mM)</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Vm</t>
   </si>
   <si>
-    <t>Kcat (min)</t>
-  </si>
-  <si>
     <t>GDK (1/10 enzyme)</t>
   </si>
   <si>
@@ -61,7 +58,13 @@
     <t>GD</t>
   </si>
   <si>
-    <t>Kcat (sec)</t>
+    <t>kcat (min)</t>
+  </si>
+  <si>
+    <t>kcat (sec)</t>
+  </si>
+  <si>
+    <t>Note: cut GGE concentration listed here is 50% of actual added amount, as stock was racemic and Lig dehydrogenases are stereospecific</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E80EE7-538F-4E48-8DC0-1C899E7A52CC}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,26 +429,31 @@
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -456,7 +464,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.1</v>
       </c>
@@ -470,7 +478,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.05</v>
       </c>
@@ -484,7 +492,7 @@
         <v>6.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -498,7 +506,7 @@
         <v>3.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -506,7 +514,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -519,8 +527,9 @@
       <c r="D10" s="1">
         <v>1.5299999999999999E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -533,10 +542,11 @@
       <c r="D11" s="1">
         <v>1.719E-6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>86.3</v>
@@ -547,8 +557,9 @@
       <c r="D12">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -557,7 +568,7 @@
         <v>1.4383333333333332</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:D13" si="0">C12/60</f>
+        <f t="shared" ref="C13:E13" si="0">C12/60</f>
         <v>0.11833333333333333</v>
       </c>
       <c r="D13">
@@ -565,12 +576,12 @@
         <v>2.8333333333333332E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -578,10 +589,10 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.2</v>
       </c>
@@ -592,7 +603,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.1</v>
       </c>
@@ -603,7 +614,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.05</v>
       </c>
@@ -614,7 +625,7 @@
         <v>6.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -625,7 +636,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -636,7 +647,7 @@
         <v>7.8999999999999996E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -647,9 +658,9 @@
         <v>1.8E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>6</v>
@@ -657,8 +668,9 @@
       <c r="C25">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -667,16 +679,16 @@
         <v>0.1</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26" si="1">C25/60</f>
+        <f t="shared" ref="C26:D26" si="1">C25/60</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -684,10 +696,10 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.2</v>
       </c>
@@ -698,7 +710,7 @@
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.1</v>
       </c>
@@ -709,7 +721,7 @@
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.05</v>
       </c>
@@ -720,7 +732,7 @@
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -731,7 +743,7 @@
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -742,7 +754,7 @@
         <v>7.2999999999999999E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -753,9 +765,9 @@
         <v>1.2E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <v>0.94</v>
@@ -763,8 +775,9 @@
       <c r="C38">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -773,7 +786,7 @@
         <v>1.5666666666666666E-2</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39" si="2">C38/60</f>
+        <f t="shared" ref="C39:D39" si="2">C38/60</f>
         <v>0.2</v>
       </c>
     </row>

</xml_diff>